<commit_message>
get started add timeline, learn : pivot table, chart
</commit_message>
<xml_diff>
--- a/get_started.xlsx
+++ b/get_started.xlsx
@@ -5,21 +5,40 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean_\Desktop\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176D63CE-380F-4FC8-961A-2985DD2D1F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B071EBF1-78D0-4276-BFD9-525753821318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" xr2:uid="{8C62D227-191E-4653-A261-C69232932DE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8C62D227-191E-4653-A261-C69232932DE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$41:$H$44</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$137:$B$139</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$136</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$137:$C$139</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$136:$C$136</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$137:$B$139</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$136</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$137:$C$139</definedName>
+    <definedName name="Slicer_Employee">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId2"/>
+  </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId3"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -37,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -653,6 +672,55 @@
   </si>
   <si>
     <t>it</t>
+  </si>
+  <si>
+    <t>7️⃣ Pivot Table (Summarize Data)</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Salary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Steps:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select the data.
+Click "Insert" → "Pivot Table" → Choose where to place it.
+Drag fields (columns) into Rows, Columns, and Values.</t>
+    </r>
+  </si>
+  <si>
+    <t>8️⃣ Charts (Visualizing Data)</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
   </si>
 </sst>
 </file>
@@ -664,7 +732,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.0_);_([$$-409]* \(#,##0.0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,6 +784,22 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -840,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -874,6 +958,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -889,67 +1031,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -978,21 +1088,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1027,6 +1137,2124 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[get_started.xlsx]Sheet1!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:softEdge rad="0"/>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="22225">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4">
+                <a:alpha val="70000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$113</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:softEdge rad="0"/>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$114:$H$116</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>HR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>IT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$114:$I$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B6C-4141-B779-89017AC0123D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:overlap val="94"/>
+        <c:axId val="973249023"/>
+        <c:axId val="973250271"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="973249023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="973250271"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="973250271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="973249023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1">
+        <a:lumMod val="50000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>sale per month</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$137:$B$139</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$137:$C$139</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CD52-4A7B-9ADB-2325017AA5E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1480037135"/>
+        <c:axId val="1480037967"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1480037135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1480037967"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1480037967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1480037135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EF63A70-8ACA-47A4-8324-9DE38460995C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>891540</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>167639</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Employee">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EFAD9A7-15F5-4F57-BB19-DAF0CE2D1C79}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Employee"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5082540" y="21496020"/>
+              <a:ext cx="1828800" cy="2263139"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>868680</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E6A8741-5F6B-405C-9E56-5C2DC01761C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="raphael Randrianantoanina" refreshedDate="45737.452284837964" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="4" xr:uid="{A829B03B-BC07-4DC5-8EE8-3411178A1621}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B113:D117" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Department" numFmtId="0">
+      <sharedItems count="2">
+        <s v="HR"/>
+        <s v="IT"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Employee" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Alice"/>
+        <s v="Bob"/>
+        <s v="John"/>
+        <s v="Emma"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Salary" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="50000" maxValue="70000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="197789609"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="4">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="50000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="60000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="55000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="70000"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B62945D-7C51-47BB-8AB8-F66FA7865570}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="H113:I116" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Salary" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Employee" xr10:uid="{8654C896-62C5-4860-ABAC-9D81FAD02184}" sourceName="Employee">
+  <pivotTables>
+    <pivotTable tabId="1" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="197789609">
+      <items count="4">
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="3" s="1"/>
+        <i x="2" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Employee" xr10:uid="{11D1B061-2750-4EDD-BF1B-C5E7C7952DF6}" cache="Slicer_Employee" caption="Employee" rowHeight="234950"/>
+</slicers>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1327,10 +3555,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBE14C7-F894-47C8-ABF5-A4FB5AA190BC}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="O136" sqref="O136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,6 +3566,7 @@
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1392,53 +3621,53 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="40">
         <f>SUM(D4:D6)</f>
         <v>165000</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="40">
         <f>MIN(D4:D6)</f>
         <v>50000</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="40">
         <f>MAX(D4:D6)</f>
         <v>60000</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="40">
         <f>AVERAGE(D4:D6)</f>
         <v>55000</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
@@ -1450,10 +3679,10 @@
       <c r="D16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -1465,11 +3694,11 @@
       <c r="D17" s="9">
         <v>5</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="37">
         <f>C17*D17</f>
         <v>50</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
@@ -1481,26 +3710,26 @@
       <c r="D18" s="9">
         <v>2</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="37">
         <f>C18*D18</f>
         <v>100</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="21" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
       <c r="E21" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
       <c r="E22" s="12"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -1544,82 +3773,82 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="15">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="15">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="15">
         <v>21</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="15">
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="41" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="24" t="s">
+      <c r="F41" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G41" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="24" t="s">
+      <c r="H41" s="16" t="s">
         <v>30</v>
       </c>
       <c r="J41" s="11" t="s">
@@ -1666,7 +3895,7 @@
       <c r="H43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J43" s="25" t="s">
+      <c r="J43" s="17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1699,30 +3928,30 @@
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="J46" s="26" t="s">
+      <c r="J46" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="D47" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G47" s="24" t="s">
+      <c r="G47" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="H47" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J47" s="26" t="s">
+      <c r="J47" s="18" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1798,7 +4027,7 @@
       <c r="J53" s="12"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="J54" s="25" t="s">
+      <c r="J54" s="17" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1818,7 +4047,7 @@
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="J58" s="25" t="s">
+      <c r="J58" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1828,193 +4057,193 @@
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B70" s="27" t="s">
+      <c r="B70" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B75" s="29" t="s">
+      <c r="B75" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="29" t="s">
+      <c r="C75" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="D75" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B76" s="22" t="s">
+      <c r="B76" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C76" s="22">
+      <c r="C76" s="15">
         <v>90</v>
       </c>
-      <c r="D76" s="22" t="str">
+      <c r="D76" s="15" t="str">
         <f>IF(C76&gt;=50, "Pass", "Fail")</f>
         <v>Pass</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C77" s="22">
+      <c r="C77" s="15">
         <v>30</v>
       </c>
-      <c r="D77" s="22" t="str">
+      <c r="D77" s="15" t="str">
         <f t="shared" ref="D77:D80" si="0">IF(C77&gt;=50, "Pass", "Fail")</f>
         <v>Fail</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B78" s="22" t="s">
+      <c r="B78" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C78" s="22">
+      <c r="C78" s="15">
         <v>80</v>
       </c>
-      <c r="D78" s="22" t="str">
+      <c r="D78" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C79" s="22">
+      <c r="C79" s="15">
         <v>28</v>
       </c>
-      <c r="D79" s="22" t="str">
+      <c r="D79" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Fail</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B80" s="22" t="s">
+      <c r="B80" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C80" s="22">
+      <c r="C80" s="15">
         <v>90</v>
       </c>
-      <c r="D80" s="22" t="str">
+      <c r="D80" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B84" s="30" t="s">
+      <c r="B84" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="34"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
+      <c r="B85" s="34"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="34"/>
     </row>
     <row r="87" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="32"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="32"/>
     </row>
     <row r="91" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="31" t="s">
+      <c r="B91" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C91" s="31" t="s">
+      <c r="C91" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E91" s="35" t="s">
+      <c r="E91" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="F91" s="36"/>
-      <c r="G91" s="33" t="s">
+      <c r="F91" s="26"/>
+      <c r="G91" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H91" s="34"/>
+      <c r="H91" s="28"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B92" s="32">
+      <c r="B92" s="21">
         <v>101</v>
       </c>
-      <c r="C92" s="32">
+      <c r="C92" s="21">
         <v>80</v>
       </c>
-      <c r="E92" s="37">
+      <c r="E92" s="29">
         <v>102</v>
       </c>
-      <c r="F92" s="37"/>
-      <c r="G92" s="37">
+      <c r="F92" s="29"/>
+      <c r="G92" s="29">
         <f>VLOOKUP(E92,$B$92:$C$94,2,FALSE)</f>
         <v>45</v>
       </c>
-      <c r="H92" s="37"/>
+      <c r="H92" s="29"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B93" s="32">
+      <c r="B93" s="21">
         <v>102</v>
       </c>
-      <c r="C93" s="32">
+      <c r="C93" s="21">
         <v>45</v>
       </c>
-      <c r="E93" s="37"/>
-      <c r="F93" s="37"/>
-      <c r="G93" s="37"/>
-      <c r="H93" s="37"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="29"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B94" s="32">
+      <c r="B94" s="21">
         <v>103</v>
       </c>
-      <c r="C94" s="32">
+      <c r="C94" s="21">
         <v>90</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B96" s="38" t="s">
+      <c r="B96" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C96" s="38" t="s">
+      <c r="C96" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F96" s="39"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="39"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23"/>
+      <c r="H96" s="23"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B97" s="2" t="s">
@@ -2026,9 +4255,9 @@
       <c r="D97" s="2">
         <v>50000</v>
       </c>
-      <c r="F97" s="40"/>
-      <c r="G97" s="40"/>
-      <c r="H97" s="40"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B98" s="2" t="s">
@@ -2064,25 +4293,25 @@
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B103" s="38" t="s">
+      <c r="B103" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C103" s="38" t="s">
+      <c r="C103" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D103" s="38" t="s">
+      <c r="D103" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B104" s="22" t="s">
+      <c r="B104" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C104" s="22" t="str">
+      <c r="C104" s="15" t="str">
         <f>VLOOKUP(B104,$B$97:$D$100,2,FALSE)</f>
         <v>Bob</v>
       </c>
-      <c r="D104" s="22">
+      <c r="D104" s="15">
         <f>VLOOKUP(C104,C97:D100,2,0)</f>
         <v>60000</v>
       </c>
@@ -2098,6 +4327,176 @@
       <c r="D107" t="e">
         <f>VLOOKUP(C107,$B$97:$D$100,2, FALSE)</f>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B110" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" s="34"/>
+      <c r="D110" s="34"/>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B111" s="34"/>
+      <c r="C111" s="34"/>
+      <c r="D111" s="34"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B113" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D113" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="H113" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="I113" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B114" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C114" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="42">
+        <v>50000</v>
+      </c>
+      <c r="H114" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="I114" s="47">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B115" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C115" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D115" s="42">
+        <v>60000</v>
+      </c>
+      <c r="H115" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="I115" s="47">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B116" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C116" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" s="42">
+        <v>55000</v>
+      </c>
+      <c r="H116" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="I116" s="47">
+        <v>235000</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B117" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C117" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D117" s="42">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B119" s="48"/>
+    </row>
+    <row r="121" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C121" s="50"/>
+      <c r="D121" s="50"/>
+      <c r="E121" s="50"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B122" s="50"/>
+      <c r="C122" s="50"/>
+      <c r="D122" s="50"/>
+      <c r="E122" s="50"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B123" s="50"/>
+      <c r="C123" s="50"/>
+      <c r="D123" s="50"/>
+      <c r="E123" s="50"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B124" s="50"/>
+      <c r="C124" s="50"/>
+      <c r="D124" s="50"/>
+      <c r="E124" s="50"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B125" s="50"/>
+      <c r="C125" s="50"/>
+      <c r="D125" s="50"/>
+      <c r="E125" s="50"/>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B133" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C133" s="34"/>
+      <c r="D133" s="34"/>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B134" s="34"/>
+      <c r="C134" s="34"/>
+      <c r="D134" s="34"/>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B136" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B137" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C137" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B138" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C138" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B139" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C139" s="2">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -2111,7 +4510,19 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F48:H50">
     <sortCondition ref="G48:G50"/>
   </sortState>
-  <mergeCells count="18">
+  <mergeCells count="21">
+    <mergeCell ref="B110:D111"/>
+    <mergeCell ref="B121:E125"/>
+    <mergeCell ref="B133:D134"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B21:D22"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="E91:F91"/>
     <mergeCell ref="G91:H91"/>
     <mergeCell ref="E92:F93"/>
@@ -2121,15 +4532,6 @@
     <mergeCell ref="B70:E71"/>
     <mergeCell ref="B84:E85"/>
     <mergeCell ref="B87:F88"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B21:D22"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
@@ -2142,11 +4544,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C35">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>20</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
-      <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
@@ -2160,6 +4562,14 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>